<commit_message>
updata DOCs for wk2 sprint2
</commit_message>
<xml_diff>
--- a/DOCs/BurnDownTeam2Wk1Sprint2.xlsx
+++ b/DOCs/BurnDownTeam2Wk1Sprint2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F95F651-CD33-4089-AE65-04D8728ECF51}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7B8056-33E7-4E8F-82F8-D3A917DF52E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32023" yWindow="891" windowWidth="24686" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36531" yWindow="1303" windowWidth="24686" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,61 +541,61 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3463,20 +3463,20 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.3828125" customWidth="1"/>
+    <col min="3" max="3" width="12.15234375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.15234375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3530,11 +3530,11 @@
         <v>31</v>
       </c>
       <c r="F3" s="4">
-        <f>$C$2-(($C$2/21)*(A2+2))</f>
+        <f t="shared" ref="F3:F21" si="1">$C$2-(($C$2/21)*(A2+2))</f>
         <v>26.571428571428569</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3548,11 +3548,11 @@
         <v>31</v>
       </c>
       <c r="F4" s="4">
-        <f>$C$2-(($C$2/21)*(A3+2))</f>
+        <f t="shared" si="1"/>
         <v>25.095238095238095</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3566,11 +3566,11 @@
         <v>31</v>
       </c>
       <c r="F5" s="4">
-        <f>$C$2-(($C$2/21)*(A4+2))</f>
+        <f t="shared" si="1"/>
         <v>23.61904761904762</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3584,11 +3584,11 @@
         <v>31</v>
       </c>
       <c r="F6" s="4">
-        <f>$C$2-(($C$2/21)*(A5+2))</f>
+        <f t="shared" si="1"/>
         <v>22.142857142857142</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3596,17 +3596,19 @@
         <v>43554</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="4">
-        <f>$C$2-(($C$2/21)*(A6+2))</f>
+        <f t="shared" si="1"/>
         <v>20.666666666666664</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3616,15 +3618,15 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E25" si="1">(E7+C8)-D8</f>
-        <v>31</v>
+        <f t="shared" ref="E8:E25" si="2">(E7+C8)-D8</f>
+        <v>30</v>
       </c>
       <c r="F8" s="4">
-        <f>$C$2-(($C$2/21)*(A7+2))</f>
+        <f t="shared" si="1"/>
         <v>19.19047619047619</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3634,15 +3636,15 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F9" s="4">
-        <f>$C$2-(($C$2/21)*(A8+2))</f>
         <v>17.714285714285715</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3652,15 +3654,15 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F10" s="4">
-        <f>$C$2-(($C$2/21)*(A9+2))</f>
         <v>16.238095238095237</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3670,15 +3672,15 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F11" s="4">
-        <f>$C$2-(($C$2/21)*(A10+2))</f>
         <v>14.761904761904759</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3688,15 +3690,15 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F12" s="4">
-        <f>$C$2-(($C$2/21)*(A11+2))</f>
         <v>13.285714285714285</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3706,15 +3708,15 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F13" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F13" s="4">
-        <f>$C$2-(($C$2/21)*(A12+2))</f>
         <v>11.80952380952381</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3724,15 +3726,15 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F14" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F14" s="4">
-        <f>$C$2-(($C$2/21)*(A13+2))</f>
         <v>10.333333333333332</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3742,15 +3744,15 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F15" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F15" s="4">
-        <f>$C$2-(($C$2/21)*(A14+2))</f>
         <v>8.8571428571428541</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3760,15 +3762,15 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F16" s="4">
-        <f>$C$2-(($C$2/21)*(A15+2))</f>
         <v>7.3809523809523796</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3778,15 +3780,15 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F17" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F17" s="4">
-        <f>$C$2-(($C$2/21)*(A16+2))</f>
         <v>5.9047619047619051</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3796,15 +3798,15 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F18" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F18" s="4">
-        <f>$C$2-(($C$2/21)*(A17+2))</f>
         <v>4.428571428571427</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3814,15 +3816,15 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F19" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F19" s="4">
-        <f>$C$2-(($C$2/21)*(A18+2))</f>
         <v>2.952380952380949</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3832,15 +3834,15 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F20" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F20" s="4">
-        <f>$C$2-(($C$2/21)*(A19+2))</f>
         <v>1.4761904761904745</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3850,15 +3852,15 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F21" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F21" s="4">
-        <f>$C$2-(($C$2/21)*(A20+2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3868,14 +3870,14 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="1">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3885,14 +3887,14 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="1">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3902,15 +3904,15 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="1">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" ref="F3:F24" si="2">$C$2-(($C$2/24)*(A23+2))</f>
+        <f t="shared" ref="F24" si="3">$C$2-(($C$2/24)*(A23+2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3920,25 +3922,25 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="1">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="F25" s="4">
         <f>$C$2-(($C$2/24)*(A24+1))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C26" s="1">
         <f>SUM(C2:C25)</f>
         <v>31</v>
       </c>
       <c r="D26" s="1">
         <f>SUM(D2:D25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>9</v>
       </c>
@@ -3964,12 +3966,12 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3980,7 +3982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3991,7 +3993,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4002,7 +4004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4013,7 +4015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4024,7 +4026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4035,7 +4037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
update DOCs for wk2 sprint2 (#22)
</commit_message>
<xml_diff>
--- a/DOCs/BurnDownTeam2Wk1Sprint2.xlsx
+++ b/DOCs/BurnDownTeam2Wk1Sprint2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F95F651-CD33-4089-AE65-04D8728ECF51}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7B8056-33E7-4E8F-82F8-D3A917DF52E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32023" yWindow="891" windowWidth="24686" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36531" yWindow="1303" windowWidth="24686" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,61 +541,61 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3463,20 +3463,20 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.3828125" customWidth="1"/>
+    <col min="3" max="3" width="12.15234375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.15234375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3530,11 +3530,11 @@
         <v>31</v>
       </c>
       <c r="F3" s="4">
-        <f>$C$2-(($C$2/21)*(A2+2))</f>
+        <f t="shared" ref="F3:F21" si="1">$C$2-(($C$2/21)*(A2+2))</f>
         <v>26.571428571428569</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3548,11 +3548,11 @@
         <v>31</v>
       </c>
       <c r="F4" s="4">
-        <f>$C$2-(($C$2/21)*(A3+2))</f>
+        <f t="shared" si="1"/>
         <v>25.095238095238095</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3566,11 +3566,11 @@
         <v>31</v>
       </c>
       <c r="F5" s="4">
-        <f>$C$2-(($C$2/21)*(A4+2))</f>
+        <f t="shared" si="1"/>
         <v>23.61904761904762</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3584,11 +3584,11 @@
         <v>31</v>
       </c>
       <c r="F6" s="4">
-        <f>$C$2-(($C$2/21)*(A5+2))</f>
+        <f t="shared" si="1"/>
         <v>22.142857142857142</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3596,17 +3596,19 @@
         <v>43554</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="4">
-        <f>$C$2-(($C$2/21)*(A6+2))</f>
+        <f t="shared" si="1"/>
         <v>20.666666666666664</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3616,15 +3618,15 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1">
-        <f t="shared" ref="E8:E25" si="1">(E7+C8)-D8</f>
-        <v>31</v>
+        <f t="shared" ref="E8:E25" si="2">(E7+C8)-D8</f>
+        <v>30</v>
       </c>
       <c r="F8" s="4">
-        <f>$C$2-(($C$2/21)*(A7+2))</f>
+        <f t="shared" si="1"/>
         <v>19.19047619047619</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3634,15 +3636,15 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F9" s="4">
-        <f>$C$2-(($C$2/21)*(A8+2))</f>
         <v>17.714285714285715</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3652,15 +3654,15 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F10" s="4">
-        <f>$C$2-(($C$2/21)*(A9+2))</f>
         <v>16.238095238095237</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3670,15 +3672,15 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F11" s="4">
-        <f>$C$2-(($C$2/21)*(A10+2))</f>
         <v>14.761904761904759</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3688,15 +3690,15 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F12" s="4">
-        <f>$C$2-(($C$2/21)*(A11+2))</f>
         <v>13.285714285714285</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3706,15 +3708,15 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F13" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F13" s="4">
-        <f>$C$2-(($C$2/21)*(A12+2))</f>
         <v>11.80952380952381</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3724,15 +3726,15 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F14" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F14" s="4">
-        <f>$C$2-(($C$2/21)*(A13+2))</f>
         <v>10.333333333333332</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3742,15 +3744,15 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F15" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F15" s="4">
-        <f>$C$2-(($C$2/21)*(A14+2))</f>
         <v>8.8571428571428541</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3760,15 +3762,15 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F16" s="4">
-        <f>$C$2-(($C$2/21)*(A15+2))</f>
         <v>7.3809523809523796</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3778,15 +3780,15 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F17" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F17" s="4">
-        <f>$C$2-(($C$2/21)*(A16+2))</f>
         <v>5.9047619047619051</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3796,15 +3798,15 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F18" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F18" s="4">
-        <f>$C$2-(($C$2/21)*(A17+2))</f>
         <v>4.428571428571427</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3814,15 +3816,15 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F19" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F19" s="4">
-        <f>$C$2-(($C$2/21)*(A18+2))</f>
         <v>2.952380952380949</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3832,15 +3834,15 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F20" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F20" s="4">
-        <f>$C$2-(($C$2/21)*(A19+2))</f>
         <v>1.4761904761904745</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3850,15 +3852,15 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="1">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F21" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="F21" s="4">
-        <f>$C$2-(($C$2/21)*(A20+2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3868,14 +3870,14 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="1">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3885,14 +3887,14 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="1">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="F23" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3902,15 +3904,15 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="1">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" ref="F3:F24" si="2">$C$2-(($C$2/24)*(A23+2))</f>
+        <f t="shared" ref="F24" si="3">$C$2-(($C$2/24)*(A23+2))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3920,25 +3922,25 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="1">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="F25" s="4">
         <f>$C$2-(($C$2/24)*(A24+1))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C26" s="1">
         <f>SUM(C2:C25)</f>
         <v>31</v>
       </c>
       <c r="D26" s="1">
         <f>SUM(D2:D25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>9</v>
       </c>
@@ -3964,12 +3966,12 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3980,7 +3982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3991,7 +3993,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4002,7 +4004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4013,7 +4015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4024,7 +4026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4035,7 +4037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added Sprint 2 docs
</commit_message>
<xml_diff>
--- a/DOCs/BurnDownTeam2Wk1Sprint2.xlsx
+++ b/DOCs/BurnDownTeam2Wk1Sprint2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7B8056-33E7-4E8F-82F8-D3A917DF52E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F441CB3-1F53-4605-A301-EDC251154D26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36531" yWindow="1303" windowWidth="24686" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="24686" windowHeight="13149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>BURN DOWN CHART      6733 Team2 Sprint1</a:t>
+              <a:t>BURN DOWN CHART      6733 Team2 Sprint2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3463,7 +3463,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>